<commit_message>
2023-03-22 fix report kdg
</commit_message>
<xml_diff>
--- a/other/완료보고서 API 김동근,박진휘.xlsx
+++ b/other/완료보고서 API 김동근,박진휘.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="132">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -323,6 +323,208 @@
   </si>
   <si>
     <t>주문 완료 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Beauty/admin/product/list</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>관리자페이지 상품목록 화면</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>상품목록 카테고리별 분류</t>
+  </si>
+  <si>
+    <t>/Beauty/admin/product/listCount</t>
+  </si>
+  <si>
+    <t>상품목록의 상품개수 세기</t>
+  </si>
+  <si>
+    <t>/Beauty/admin/product/register</t>
+  </si>
+  <si>
+    <t>관리자페이지 상품등록 화면</t>
+  </si>
+  <si>
+    <t>상품,추가옵션 등록</t>
+  </si>
+  <si>
+    <t>/Beauty/admin/product/list/delete</t>
+  </si>
+  <si>
+    <t>삭제버튼을 이용한 상품삭제</t>
+  </si>
+  <si>
+    <t>체크박스를 이용한 상품삭제</t>
+  </si>
+  <si>
+    <t>/Beauty/admin/product/search</t>
+  </si>
+  <si>
+    <t>관리자페이지 상품검색화면</t>
+  </si>
+  <si>
+    <t>어드민</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멤버</t>
+  </si>
+  <si>
+    <t>회원가입</t>
+  </si>
+  <si>
+    <t>/Beauty/member/login</t>
+  </si>
+  <si>
+    <t>로그인</t>
+  </si>
+  <si>
+    <t>/Beauty/member/find?type=1</t>
+  </si>
+  <si>
+    <t>아이디 찾기</t>
+  </si>
+  <si>
+    <t>/Beauty/member/find?type=2</t>
+  </si>
+  <si>
+    <t>비밀번호 찾기</t>
+  </si>
+  <si>
+    <t>/Beauty/member/findIdResult</t>
+  </si>
+  <si>
+    <t>/Beauty/member/findPwResult</t>
+  </si>
+  <si>
+    <t>비밀번호 변경</t>
+  </si>
+  <si>
+    <t>상품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Beauty/member/register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Beauty/shop/list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 목록 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Beauty/shop/view</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Beauty/addWish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위시리스트 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Beauty/addCart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Beauty/addOrder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고객센터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요구사항명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상세설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>특이사항</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멤버</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멤버로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인창동적처리, 비밀번호 보이기 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Member_findID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Member_login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디 찾기 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이메일인증으로 찾기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -331,7 +533,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
+    <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -384,11 +586,29 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
@@ -677,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -688,9 +908,14 @@
     <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.875" customWidth="1"/>
     <col min="4" max="4" width="23.875" customWidth="1"/>
+    <col min="6" max="6" width="12.75" customWidth="1"/>
+    <col min="7" max="7" width="16.375" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="29.875" customWidth="1"/>
+    <col min="10" max="10" width="34.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -703,8 +928,27 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F1" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1">
+        <f>+N:N</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -713,8 +957,24 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -724,13 +984,25 @@
       <c r="D3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>43</v>
       </c>
@@ -741,340 +1013,595 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>26</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
-        <v>3</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" t="s">
-        <v>57</v>
-      </c>
+      <c r="A29" s="9">
+        <v>4</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="D30" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>5</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
         <v>62</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C45" t="s">
         <v>11</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D45" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
         <v>64</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C46" t="s">
         <v>12</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D46" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
         <v>67</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C47" t="s">
         <v>69</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D47" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
         <v>68</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C48" t="s">
         <v>69</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D48" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
         <v>72</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C49" t="s">
         <v>73</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D49" t="s">
         <v>74</v>
       </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="5">
+        <v>6</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B51" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B52" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B53" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B54" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B55" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B56" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B57" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B58" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="9">
+        <v>7</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>